<commit_message>
fixed error in abbreviation name
</commit_message>
<xml_diff>
--- a/tables/table5.xlsx
+++ b/tables/table5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>88-soil</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>ucrss_fast_wfilter</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -561,14 +558,14 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
+      <c r="B11" s="2">
+        <v>1525</v>
+      </c>
+      <c r="C11" s="2">
+        <v>52811</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>